<commit_message>
almost done 2 flies left to clean
</commit_message>
<xml_diff>
--- a/labelled_csv_files/labelled_M_0030_17y9m_1_fa.xlsx
+++ b/labelled_csv_files/labelled_M_0030_17y9m_1_fa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shababayub/go/src/github.com/s4ayub/fydp/labelled_csv_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahul/Documents/fydp/labelled_csv_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A79FA4-E440-0D4C-BE9A-B652467EB1A4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{66FA5EBA-18BD-8346-B339-76E02E8BBBE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="10540" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="labelled_M_0030_17y9m_1_fa" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="980" uniqueCount="515">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="980" uniqueCount="514">
   <si>
     <t>title</t>
   </si>
@@ -595,9 +595,6 @@
   </si>
   <si>
     <t>p000001s000001w000109</t>
-  </si>
-  <si>
-    <t>AN</t>
   </si>
   <si>
     <t>p000001s000001w000110</t>
@@ -1575,7 +1572,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2418,11 +2415,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109:F110"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="C307" activeCellId="1" sqref="D109:F110 C307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4615,10 +4612,10 @@
         <v>44.48</v>
       </c>
       <c r="D110" s="1">
-        <v>44.704999999999998</v>
+        <v>44.48</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>51</v>
@@ -4629,7 +4626,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C111">
         <v>44.704999999999998</v>
@@ -4638,7 +4635,7 @@
         <v>44.905000000000001</v>
       </c>
       <c r="E111" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F111" t="s">
         <v>7</v>
@@ -4649,7 +4646,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C112">
         <v>44.905000000000001</v>
@@ -4658,7 +4655,7 @@
         <v>45.39</v>
       </c>
       <c r="E112" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F112" t="s">
         <v>7</v>
@@ -4669,7 +4666,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C113">
         <v>45.39</v>
@@ -4689,7 +4686,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C114">
         <v>45.42</v>
@@ -4709,7 +4706,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C115">
         <v>45.534999999999997</v>
@@ -4729,7 +4726,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C116">
         <v>45.63</v>
@@ -4738,7 +4735,7 @@
         <v>45.914999999999999</v>
       </c>
       <c r="E116" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F116" t="s">
         <v>7</v>
@@ -4749,7 +4746,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C117">
         <v>45.914999999999999</v>
@@ -4758,7 +4755,7 @@
         <v>46.115000000000002</v>
       </c>
       <c r="E117" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F117" t="s">
         <v>7</v>
@@ -4769,7 +4766,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C118">
         <v>46.115000000000002</v>
@@ -4778,7 +4775,7 @@
         <v>46.15</v>
       </c>
       <c r="E118" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F118" t="s">
         <v>7</v>
@@ -4789,7 +4786,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C119">
         <v>46.15</v>
@@ -4798,7 +4795,7 @@
         <v>47.43</v>
       </c>
       <c r="E119" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F119" t="s">
         <v>7</v>
@@ -4809,7 +4806,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C120">
         <v>47.43</v>
@@ -4829,7 +4826,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C121">
         <v>48.064999999999998</v>
@@ -4849,7 +4846,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C122">
         <v>50.354999999999997</v>
@@ -4858,7 +4855,7 @@
         <v>50.53</v>
       </c>
       <c r="E122" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F122" t="s">
         <v>7</v>
@@ -4869,7 +4866,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C123">
         <v>50.53</v>
@@ -4889,7 +4886,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C124">
         <v>50.585000000000001</v>
@@ -4898,7 +4895,7 @@
         <v>50.95</v>
       </c>
       <c r="E124" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F124" t="s">
         <v>7</v>
@@ -4909,7 +4906,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C125">
         <v>50.95</v>
@@ -4918,7 +4915,7 @@
         <v>51.36</v>
       </c>
       <c r="E125" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F125" t="s">
         <v>7</v>
@@ -4929,7 +4926,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C126">
         <v>51.36</v>
@@ -4938,7 +4935,7 @@
         <v>51.68</v>
       </c>
       <c r="E126" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F126" t="s">
         <v>7</v>
@@ -4949,7 +4946,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C127">
         <v>51.68</v>
@@ -4958,7 +4955,7 @@
         <v>51.975000000000001</v>
       </c>
       <c r="E127" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F127" t="s">
         <v>7</v>
@@ -4969,7 +4966,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C128">
         <v>51.975000000000001</v>
@@ -4978,7 +4975,7 @@
         <v>52.24</v>
       </c>
       <c r="E128" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F128" t="s">
         <v>7</v>
@@ -4989,7 +4986,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C129">
         <v>52.24</v>
@@ -5009,7 +5006,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C130">
         <v>52.37</v>
@@ -5018,7 +5015,7 @@
         <v>52.72</v>
       </c>
       <c r="E130" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F130" t="s">
         <v>7</v>
@@ -5029,7 +5026,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C131">
         <v>52.72</v>
@@ -5038,7 +5035,7 @@
         <v>52.954999999999998</v>
       </c>
       <c r="E131" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F131" t="s">
         <v>7</v>
@@ -5049,7 +5046,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C132">
         <v>52.954999999999998</v>
@@ -5058,7 +5055,7 @@
         <v>53.17</v>
       </c>
       <c r="E132" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F132" t="s">
         <v>7</v>
@@ -5069,7 +5066,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C133">
         <v>53.17</v>
@@ -5089,7 +5086,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C134">
         <v>53.325000000000003</v>
@@ -5098,7 +5095,7 @@
         <v>53.465000000000003</v>
       </c>
       <c r="E134" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F134" t="s">
         <v>7</v>
@@ -5109,7 +5106,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C135">
         <v>53.465000000000003</v>
@@ -5118,7 +5115,7 @@
         <v>53.49</v>
       </c>
       <c r="E135" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F135" t="s">
         <v>7</v>
@@ -5129,7 +5126,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C136">
         <v>53.49</v>
@@ -5149,7 +5146,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C137">
         <v>53.52</v>
@@ -5169,7 +5166,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C138">
         <v>53.645000000000003</v>
@@ -5178,7 +5175,7 @@
         <v>54.85</v>
       </c>
       <c r="E138" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F138" t="s">
         <v>7</v>
@@ -5189,7 +5186,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C139">
         <v>54.85</v>
@@ -5209,7 +5206,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C140">
         <v>55.68</v>
@@ -5229,7 +5226,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C141">
         <v>57.83</v>
@@ -5238,7 +5235,7 @@
         <v>58.1</v>
       </c>
       <c r="E141" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F141" t="s">
         <v>7</v>
@@ -5249,7 +5246,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C142">
         <v>58.1</v>
@@ -5258,7 +5255,7 @@
         <v>58.424999999999997</v>
       </c>
       <c r="E142" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F142" t="s">
         <v>7</v>
@@ -5269,7 +5266,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C143">
         <v>58.424999999999997</v>
@@ -5289,7 +5286,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C144">
         <v>58.475000000000001</v>
@@ -5298,7 +5295,7 @@
         <v>58.65</v>
       </c>
       <c r="E144" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F144" t="s">
         <v>7</v>
@@ -5309,7 +5306,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C145">
         <v>58.65</v>
@@ -5318,7 +5315,7 @@
         <v>59.75</v>
       </c>
       <c r="E145" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F145" t="s">
         <v>7</v>
@@ -5329,7 +5326,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C146">
         <v>59.75</v>
@@ -5349,7 +5346,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C147">
         <v>59.9</v>
@@ -5358,7 +5355,7 @@
         <v>60.06</v>
       </c>
       <c r="E147" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F147" t="s">
         <v>7</v>
@@ -5369,7 +5366,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C148">
         <v>60.06</v>
@@ -5378,7 +5375,7 @@
         <v>60.244999999999997</v>
       </c>
       <c r="E148" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F148" t="s">
         <v>7</v>
@@ -5389,7 +5386,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C149">
         <v>60.244999999999997</v>
@@ -5398,7 +5395,7 @@
         <v>60.604999999999997</v>
       </c>
       <c r="E149" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F149" t="s">
         <v>7</v>
@@ -5409,7 +5406,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C150">
         <v>60.604999999999997</v>
@@ -5429,7 +5426,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C151">
         <v>62.534999999999997</v>
@@ -5449,7 +5446,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C152">
         <v>62.83</v>
@@ -5469,7 +5466,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C153">
         <v>62.89</v>
@@ -5478,7 +5475,7 @@
         <v>63.17</v>
       </c>
       <c r="E153" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F153" t="s">
         <v>7</v>
@@ -5489,7 +5486,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C154">
         <v>63.17</v>
@@ -5498,7 +5495,7 @@
         <v>63.49</v>
       </c>
       <c r="E154" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F154" t="s">
         <v>7</v>
@@ -5509,7 +5506,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C155">
         <v>63.49</v>
@@ -5518,7 +5515,7 @@
         <v>63.72</v>
       </c>
       <c r="E155" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F155" t="s">
         <v>7</v>
@@ -5529,7 +5526,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C156">
         <v>63.72</v>
@@ -5549,7 +5546,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C157">
         <v>63.93</v>
@@ -5558,7 +5555,7 @@
         <v>64.144999999999996</v>
       </c>
       <c r="E157" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F157" t="s">
         <v>7</v>
@@ -5569,7 +5566,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C158">
         <v>64.144999999999996</v>
@@ -5578,7 +5575,7 @@
         <v>65.52</v>
       </c>
       <c r="E158" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F158" t="s">
         <v>94</v>
@@ -5589,7 +5586,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C159">
         <v>65.52</v>
@@ -5598,7 +5595,7 @@
         <v>65.555000000000007</v>
       </c>
       <c r="E159" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F159" t="s">
         <v>7</v>
@@ -5609,7 +5606,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C160">
         <v>65.555000000000007</v>
@@ -5618,7 +5615,7 @@
         <v>66.284999999999997</v>
       </c>
       <c r="E160" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F160" t="s">
         <v>7</v>
@@ -5629,7 +5626,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C161">
         <v>66.284999999999997</v>
@@ -5649,7 +5646,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C162">
         <v>66.459999999999994</v>
@@ -5658,7 +5655,7 @@
         <v>66.875</v>
       </c>
       <c r="E162" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F162" t="s">
         <v>7</v>
@@ -5669,7 +5666,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C163">
         <v>66.875</v>
@@ -5678,7 +5675,7 @@
         <v>67.88</v>
       </c>
       <c r="E163" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F163" t="s">
         <v>7</v>
@@ -5689,7 +5686,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C164">
         <v>67.88</v>
@@ -5698,7 +5695,7 @@
         <v>68.415000000000006</v>
       </c>
       <c r="E164" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F164" t="s">
         <v>7</v>
@@ -5709,7 +5706,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C165">
         <v>68.415000000000006</v>
@@ -5729,7 +5726,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C166">
         <v>68.474999999999994</v>
@@ -5738,7 +5735,7 @@
         <v>68.97</v>
       </c>
       <c r="E166" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F166" t="s">
         <v>7</v>
@@ -5749,7 +5746,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C167">
         <v>68.97</v>
@@ -5758,7 +5755,7 @@
         <v>69.545000000000002</v>
       </c>
       <c r="E167" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F167" t="s">
         <v>7</v>
@@ -5769,7 +5766,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C168">
         <v>69.545000000000002</v>
@@ -5778,7 +5775,7 @@
         <v>69.64</v>
       </c>
       <c r="E168" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F168" t="s">
         <v>7</v>
@@ -5789,7 +5786,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C169">
         <v>69.64</v>
@@ -5809,7 +5806,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C170">
         <v>69.81</v>
@@ -5829,7 +5826,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C171">
         <v>69.894999999999996</v>
@@ -5849,7 +5846,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C172">
         <v>70.069999999999993</v>
@@ -5858,7 +5855,7 @@
         <v>70.254999999999995</v>
       </c>
       <c r="E172" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F172" t="s">
         <v>7</v>
@@ -5869,7 +5866,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C173">
         <v>70.254999999999995</v>
@@ -5878,7 +5875,7 @@
         <v>70.569999999999993</v>
       </c>
       <c r="E173" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F173" t="s">
         <v>7</v>
@@ -5889,7 +5886,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C174">
         <v>70.569999999999993</v>
@@ -5898,7 +5895,7 @@
         <v>71.155000000000001</v>
       </c>
       <c r="E174" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F174" t="s">
         <v>7</v>
@@ -5909,7 +5906,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C175">
         <v>71.155000000000001</v>
@@ -5929,7 +5926,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C176">
         <v>72.305000000000007</v>
@@ -5949,7 +5946,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C177">
         <v>72.53</v>
@@ -5958,7 +5955,7 @@
         <v>72.69</v>
       </c>
       <c r="E177" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F177" t="s">
         <v>7</v>
@@ -5969,7 +5966,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C178">
         <v>72.69</v>
@@ -5989,7 +5986,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C179">
         <v>72.78</v>
@@ -6009,7 +6006,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C180">
         <v>72.784999999999997</v>
@@ -6029,7 +6026,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C181">
         <v>73.02</v>
@@ -6049,7 +6046,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C182">
         <v>73.03</v>
@@ -6058,7 +6055,7 @@
         <v>74.094999999999999</v>
       </c>
       <c r="E182" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F182" t="s">
         <v>7</v>
@@ -6069,7 +6066,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C183">
         <v>74.094999999999999</v>
@@ -6089,7 +6086,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C184">
         <v>74.655000000000001</v>
@@ -6098,7 +6095,7 @@
         <v>74.905000000000001</v>
       </c>
       <c r="E184" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F184" t="s">
         <v>7</v>
@@ -6109,7 +6106,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C185">
         <v>74.905000000000001</v>
@@ -6129,7 +6126,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C186">
         <v>74.944999999999993</v>
@@ -6138,7 +6135,7 @@
         <v>75.010000000000005</v>
       </c>
       <c r="E186" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F186" t="s">
         <v>7</v>
@@ -6149,7 +6146,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C187">
         <v>75.010000000000005</v>
@@ -6158,7 +6155,7 @@
         <v>75.265000000000001</v>
       </c>
       <c r="E187" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F187" t="s">
         <v>7</v>
@@ -6169,7 +6166,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C188">
         <v>75.265000000000001</v>
@@ -6189,7 +6186,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C189">
         <v>75.72</v>
@@ -6198,7 +6195,7 @@
         <v>76.474999999999994</v>
       </c>
       <c r="E189" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F189" t="s">
         <v>7</v>
@@ -6209,7 +6206,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C190">
         <v>76.474999999999994</v>
@@ -6229,7 +6226,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C191">
         <v>76.614999999999995</v>
@@ -6238,7 +6235,7 @@
         <v>76.974999999999994</v>
       </c>
       <c r="E191" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F191" t="s">
         <v>7</v>
@@ -6249,7 +6246,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C192">
         <v>76.974999999999994</v>
@@ -6258,7 +6255,7 @@
         <v>77.305000000000007</v>
       </c>
       <c r="E192" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F192" t="s">
         <v>7</v>
@@ -6269,7 +6266,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C193">
         <v>77.305000000000007</v>
@@ -6278,7 +6275,7 @@
         <v>77.5</v>
       </c>
       <c r="E193" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F193" t="s">
         <v>7</v>
@@ -6289,7 +6286,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C194">
         <v>77.5</v>
@@ -6298,7 +6295,7 @@
         <v>78.58</v>
       </c>
       <c r="E194" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F194" t="s">
         <v>7</v>
@@ -6309,7 +6306,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C195">
         <v>78.58</v>
@@ -6318,7 +6315,7 @@
         <v>78.91</v>
       </c>
       <c r="E195" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F195" t="s">
         <v>28</v>
@@ -6329,7 +6326,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C196">
         <v>78.91</v>
@@ -6338,7 +6335,7 @@
         <v>79.45</v>
       </c>
       <c r="E196" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F196" t="s">
         <v>7</v>
@@ -6349,7 +6346,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C197">
         <v>79.45</v>
@@ -6358,7 +6355,7 @@
         <v>79.454999999999998</v>
       </c>
       <c r="E197" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F197" t="s">
         <v>7</v>
@@ -6369,7 +6366,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C198">
         <v>79.454999999999998</v>
@@ -6389,7 +6386,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C199">
         <v>79.454999999999998</v>
@@ -6409,7 +6406,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C200">
         <v>79.694999999999993</v>
@@ -6429,7 +6426,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C201">
         <v>80.09</v>
@@ -6449,7 +6446,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C202">
         <v>80.105000000000004</v>
@@ -6458,7 +6455,7 @@
         <v>80.53</v>
       </c>
       <c r="E202" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F202" t="s">
         <v>7</v>
@@ -6469,7 +6466,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C203">
         <v>80.53</v>
@@ -6478,7 +6475,7 @@
         <v>80.95</v>
       </c>
       <c r="E203" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F203" t="s">
         <v>7</v>
@@ -6489,7 +6486,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C204">
         <v>80.95</v>
@@ -6498,7 +6495,7 @@
         <v>81.12</v>
       </c>
       <c r="E204" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F204" t="s">
         <v>7</v>
@@ -6509,7 +6506,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C205">
         <v>81.12</v>
@@ -6518,7 +6515,7 @@
         <v>81.474999999999994</v>
       </c>
       <c r="E205" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F205" t="s">
         <v>7</v>
@@ -6529,7 +6526,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C206">
         <v>81.474999999999994</v>
@@ -6538,7 +6535,7 @@
         <v>81.734999999999999</v>
       </c>
       <c r="E206" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F206" t="s">
         <v>7</v>
@@ -6549,7 +6546,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C207">
         <v>81.734999999999999</v>
@@ -6569,7 +6566,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C208">
         <v>81.974999999999994</v>
@@ -6578,7 +6575,7 @@
         <v>82.504999999999995</v>
       </c>
       <c r="E208" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F208" t="s">
         <v>7</v>
@@ -6589,7 +6586,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C209">
         <v>82.504999999999995</v>
@@ -6598,7 +6595,7 @@
         <v>83.02</v>
       </c>
       <c r="E209" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F209" t="s">
         <v>7</v>
@@ -6609,7 +6606,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C210">
         <v>83.02</v>
@@ -6618,10 +6615,10 @@
         <v>83.125</v>
       </c>
       <c r="E210" t="s">
+        <v>347</v>
+      </c>
+      <c r="F210" t="s">
         <v>348</v>
-      </c>
-      <c r="F210" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
@@ -6629,7 +6626,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C211">
         <v>83.125</v>
@@ -6638,10 +6635,10 @@
         <v>83.555000000000007</v>
       </c>
       <c r="E211" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F211" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
@@ -6649,7 +6646,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C212">
         <v>83.555000000000007</v>
@@ -6658,10 +6655,10 @@
         <v>84.465000000000003</v>
       </c>
       <c r="E212" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F212" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
@@ -6669,7 +6666,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C213">
         <v>84.465000000000003</v>
@@ -6678,10 +6675,10 @@
         <v>84.52</v>
       </c>
       <c r="E213" t="s">
+        <v>347</v>
+      </c>
+      <c r="F213" t="s">
         <v>348</v>
-      </c>
-      <c r="F213" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
@@ -6689,7 +6686,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C214">
         <v>84.52</v>
@@ -6698,10 +6695,10 @@
         <v>84.704999999999998</v>
       </c>
       <c r="E214" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F214" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
@@ -6709,7 +6706,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C215">
         <v>84.704999999999998</v>
@@ -6729,7 +6726,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C216">
         <v>84.91</v>
@@ -6738,7 +6735,7 @@
         <v>85.62</v>
       </c>
       <c r="E216" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F216" t="s">
         <v>7</v>
@@ -6749,7 +6746,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C217">
         <v>85.62</v>
@@ -6769,7 +6766,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C218">
         <v>86.47</v>
@@ -6789,7 +6786,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C219">
         <v>86.625</v>
@@ -6798,7 +6795,7 @@
         <v>86.635000000000005</v>
       </c>
       <c r="E219" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F219" t="s">
         <v>7</v>
@@ -6809,7 +6806,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C220">
         <v>86.635000000000005</v>
@@ -6818,7 +6815,7 @@
         <v>87.14</v>
       </c>
       <c r="E220" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F220" t="s">
         <v>7</v>
@@ -6829,7 +6826,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C221">
         <v>87.14</v>
@@ -6838,7 +6835,7 @@
         <v>87.32</v>
       </c>
       <c r="E221" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F221" t="s">
         <v>7</v>
@@ -6849,7 +6846,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C222">
         <v>87.32</v>
@@ -6869,7 +6866,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C223">
         <v>87.47</v>
@@ -6889,7 +6886,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C224">
         <v>87.53</v>
@@ -6898,7 +6895,7 @@
         <v>87.68</v>
       </c>
       <c r="E224" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F224" t="s">
         <v>7</v>
@@ -6909,7 +6906,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C225">
         <v>87.68</v>
@@ -6918,7 +6915,7 @@
         <v>87.855000000000004</v>
       </c>
       <c r="E225" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F225" t="s">
         <v>7</v>
@@ -6929,7 +6926,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C226">
         <v>87.855000000000004</v>
@@ -6949,7 +6946,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C227">
         <v>88.025000000000006</v>
@@ -6969,7 +6966,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C228">
         <v>88.03</v>
@@ -6978,7 +6975,7 @@
         <v>88.185000000000002</v>
       </c>
       <c r="E228" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F228" t="s">
         <v>7</v>
@@ -6989,7 +6986,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C229">
         <v>88.185000000000002</v>
@@ -6998,7 +6995,7 @@
         <v>89.5</v>
       </c>
       <c r="E229" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F229" t="s">
         <v>7</v>
@@ -7009,7 +7006,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C230">
         <v>89.5</v>
@@ -7029,7 +7026,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C231">
         <v>90.37</v>
@@ -7049,7 +7046,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C232">
         <v>90.57</v>
@@ -7058,7 +7055,7 @@
         <v>90.644999999999996</v>
       </c>
       <c r="E232" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F232" t="s">
         <v>7</v>
@@ -7069,7 +7066,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C233">
         <v>90.644999999999996</v>
@@ -7089,7 +7086,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C234">
         <v>90.69</v>
@@ -7109,7 +7106,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C235">
         <v>90.885000000000005</v>
@@ -7118,7 +7115,7 @@
         <v>93.004999999999995</v>
       </c>
       <c r="E235" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F235" t="s">
         <v>28</v>
@@ -7129,7 +7126,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C236">
         <v>93.004999999999995</v>
@@ -7138,7 +7135,7 @@
         <v>93.174999999999997</v>
       </c>
       <c r="E236" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F236" t="s">
         <v>7</v>
@@ -7149,7 +7146,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C237">
         <v>93.174999999999997</v>
@@ -7158,7 +7155,7 @@
         <v>93.48</v>
       </c>
       <c r="E237" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F237" t="s">
         <v>7</v>
@@ -7169,7 +7166,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C238">
         <v>93.48</v>
@@ -7189,7 +7186,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C239">
         <v>93.55</v>
@@ -7209,7 +7206,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C240">
         <v>93.63</v>
@@ -7229,7 +7226,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C241">
         <v>93.935000000000002</v>
@@ -7238,7 +7235,7 @@
         <v>94.28</v>
       </c>
       <c r="E241" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F241" t="s">
         <v>7</v>
@@ -7249,7 +7246,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C242">
         <v>94.28</v>
@@ -7258,7 +7255,7 @@
         <v>95.08</v>
       </c>
       <c r="E242" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F242" t="s">
         <v>7</v>
@@ -7269,7 +7266,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C243">
         <v>95.08</v>
@@ -7289,7 +7286,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C244">
         <v>95.9</v>
@@ -7298,7 +7295,7 @@
         <v>96.06</v>
       </c>
       <c r="E244" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F244" t="s">
         <v>7</v>
@@ -7309,7 +7306,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C245">
         <v>96.06</v>
@@ -7329,7 +7326,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C246">
         <v>96.63</v>
@@ -7349,7 +7346,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C247">
         <v>96.72</v>
@@ -7358,7 +7355,7 @@
         <v>96.94</v>
       </c>
       <c r="E247" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F247" t="s">
         <v>7</v>
@@ -7369,7 +7366,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C248">
         <v>96.94</v>
@@ -7378,7 +7375,7 @@
         <v>97.11</v>
       </c>
       <c r="E248" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F248" t="s">
         <v>7</v>
@@ -7389,7 +7386,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C249">
         <v>97.11</v>
@@ -7398,7 +7395,7 @@
         <v>97.3</v>
       </c>
       <c r="E249" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F249" t="s">
         <v>7</v>
@@ -7409,7 +7406,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C250">
         <v>97.3</v>
@@ -7418,7 +7415,7 @@
         <v>97.48</v>
       </c>
       <c r="E250" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F250" t="s">
         <v>7</v>
@@ -7429,7 +7426,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C251">
         <v>97.48</v>
@@ -7438,7 +7435,7 @@
         <v>97.594999999999999</v>
       </c>
       <c r="E251" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F251" t="s">
         <v>7</v>
@@ -7449,7 +7446,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C252">
         <v>97.594999999999999</v>
@@ -7458,7 +7455,7 @@
         <v>98.05</v>
       </c>
       <c r="E252" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F252" t="s">
         <v>7</v>
@@ -7469,7 +7466,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C253">
         <v>98.05</v>
@@ -7478,7 +7475,7 @@
         <v>98.4</v>
       </c>
       <c r="E253" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F253" t="s">
         <v>7</v>
@@ -7489,7 +7486,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C254">
         <v>98.4</v>
@@ -7509,7 +7506,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C255">
         <v>98.45</v>
@@ -7518,7 +7515,7 @@
         <v>98.625</v>
       </c>
       <c r="E255" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F255" t="s">
         <v>7</v>
@@ -7529,7 +7526,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C256">
         <v>98.625</v>
@@ -7538,7 +7535,7 @@
         <v>98.825000000000003</v>
       </c>
       <c r="E256" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F256" t="s">
         <v>7</v>
@@ -7549,7 +7546,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C257">
         <v>98.825000000000003</v>
@@ -7558,7 +7555,7 @@
         <v>99.18</v>
       </c>
       <c r="E257" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F257" t="s">
         <v>7</v>
@@ -7569,7 +7566,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C258">
         <v>99.18</v>
@@ -7578,7 +7575,7 @@
         <v>99.26</v>
       </c>
       <c r="E258" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F258" t="s">
         <v>7</v>
@@ -7589,7 +7586,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C259">
         <v>99.26</v>
@@ -7609,7 +7606,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C260">
         <v>100.705</v>
@@ -7618,7 +7615,7 @@
         <v>100.97</v>
       </c>
       <c r="E260" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F260" t="s">
         <v>7</v>
@@ -7629,7 +7626,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C261">
         <v>100.97</v>
@@ -7649,7 +7646,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C262">
         <v>101.08499999999999</v>
@@ -7669,7 +7666,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C263">
         <v>101.325</v>
@@ -7689,7 +7686,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C264">
         <v>101.66500000000001</v>
@@ -7709,7 +7706,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C265">
         <v>101.85</v>
@@ -7718,7 +7715,7 @@
         <v>102.285</v>
       </c>
       <c r="E265" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F265" t="s">
         <v>7</v>
@@ -7729,7 +7726,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C266">
         <v>102.285</v>
@@ -7738,7 +7735,7 @@
         <v>102.895</v>
       </c>
       <c r="E266" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F266" t="s">
         <v>7</v>
@@ -7749,7 +7746,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C267">
         <v>102.895</v>
@@ -7769,7 +7766,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C268">
         <v>103.38</v>
@@ -7789,7 +7786,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C269">
         <v>103.625</v>
@@ -7798,7 +7795,7 @@
         <v>103.8</v>
       </c>
       <c r="E269" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F269" t="s">
         <v>7</v>
@@ -7809,7 +7806,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C270">
         <v>103.8</v>
@@ -7818,7 +7815,7 @@
         <v>104.08499999999999</v>
       </c>
       <c r="E270" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F270" t="s">
         <v>7</v>
@@ -7829,7 +7826,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C271">
         <v>104.08499999999999</v>
@@ -7849,7 +7846,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C272">
         <v>104.62</v>
@@ -7858,7 +7855,7 @@
         <v>105.005</v>
       </c>
       <c r="E272" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F272" t="s">
         <v>7</v>
@@ -7869,7 +7866,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C273">
         <v>105.005</v>
@@ -7878,7 +7875,7 @@
         <v>105.14</v>
       </c>
       <c r="E273" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F273" t="s">
         <v>7</v>
@@ -7889,7 +7886,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C274">
         <v>105.14</v>
@@ -7909,7 +7906,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C275">
         <v>105.235</v>
@@ -7918,7 +7915,7 @@
         <v>105.61</v>
       </c>
       <c r="E275" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F275" t="s">
         <v>7</v>
@@ -7929,7 +7926,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C276">
         <v>105.61</v>
@@ -7938,7 +7935,7 @@
         <v>105.77500000000001</v>
       </c>
       <c r="E276" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F276" t="s">
         <v>7</v>
@@ -7949,7 +7946,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C277">
         <v>105.77500000000001</v>
@@ -7958,7 +7955,7 @@
         <v>107.04</v>
       </c>
       <c r="E277" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F277" t="s">
         <v>7</v>
@@ -7969,7 +7966,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C278">
         <v>107.04</v>
@@ -7989,7 +7986,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C279">
         <v>108.83499999999999</v>
@@ -7998,7 +7995,7 @@
         <v>109.435</v>
       </c>
       <c r="E279" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F279" t="s">
         <v>7</v>
@@ -8009,7 +8006,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C280">
         <v>109.435</v>
@@ -8018,7 +8015,7 @@
         <v>109.65</v>
       </c>
       <c r="E280" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F280" t="s">
         <v>7</v>
@@ -8029,7 +8026,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C281">
         <v>109.65</v>
@@ -8038,7 +8035,7 @@
         <v>110.145</v>
       </c>
       <c r="E281" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F281" t="s">
         <v>7</v>
@@ -8049,7 +8046,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C282">
         <v>110.145</v>
@@ -8058,7 +8055,7 @@
         <v>111.815</v>
       </c>
       <c r="E282" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F282" t="s">
         <v>7</v>
@@ -8069,7 +8066,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C283">
         <v>111.815</v>
@@ -8078,7 +8075,7 @@
         <v>113.825</v>
       </c>
       <c r="E283" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F283" t="s">
         <v>28</v>
@@ -8089,7 +8086,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C284">
         <v>113.825</v>
@@ -8109,7 +8106,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C285">
         <v>113.95</v>
@@ -8118,7 +8115,7 @@
         <v>114.14</v>
       </c>
       <c r="E285" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F285" t="s">
         <v>7</v>
@@ -8129,7 +8126,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C286">
         <v>114.14</v>
@@ -8138,7 +8135,7 @@
         <v>114.37</v>
       </c>
       <c r="E286" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F286" t="s">
         <v>7</v>
@@ -8149,7 +8146,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C287">
         <v>114.37</v>
@@ -8169,7 +8166,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C288">
         <v>114.64</v>
@@ -8178,7 +8175,7 @@
         <v>115.1</v>
       </c>
       <c r="E288" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F288" t="s">
         <v>7</v>
@@ -8189,7 +8186,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C289">
         <v>115.1</v>
@@ -8209,7 +8206,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C290">
         <v>115.605</v>
@@ -8229,7 +8226,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C291">
         <v>115.80500000000001</v>
@@ -8238,7 +8235,7 @@
         <v>115.83499999999999</v>
       </c>
       <c r="E291" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F291" t="s">
         <v>7</v>
@@ -8249,7 +8246,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C292">
         <v>115.83499999999999</v>
@@ -8258,7 +8255,7 @@
         <v>115.83499999999999</v>
       </c>
       <c r="E292" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F292" t="s">
         <v>7</v>
@@ -8269,7 +8266,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C293">
         <v>115.83499999999999</v>
@@ -8289,7 +8286,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C294">
         <v>115.83499999999999</v>
@@ -8298,7 +8295,7 @@
         <v>115.97499999999999</v>
       </c>
       <c r="E294" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F294" t="s">
         <v>7</v>
@@ -8309,7 +8306,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C295">
         <v>115.97499999999999</v>
@@ -8329,7 +8326,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C296">
         <v>116.295</v>
@@ -8349,7 +8346,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C297">
         <v>116.33</v>
@@ -8358,7 +8355,7 @@
         <v>116.53</v>
       </c>
       <c r="E297" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F297" t="s">
         <v>7</v>
@@ -8369,7 +8366,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C298">
         <v>116.53</v>
@@ -8378,7 +8375,7 @@
         <v>117.41500000000001</v>
       </c>
       <c r="E298" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F298" t="s">
         <v>7</v>
@@ -8389,7 +8386,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C299">
         <v>117.41500000000001</v>
@@ -8398,7 +8395,7 @@
         <v>118.45</v>
       </c>
       <c r="E299" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F299" t="s">
         <v>94</v>
@@ -8409,7 +8406,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C300">
         <v>118.45</v>
@@ -8418,7 +8415,7 @@
         <v>118.97499999999999</v>
       </c>
       <c r="E300" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F300" t="s">
         <v>7</v>
@@ -8429,7 +8426,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C301">
         <v>118.97499999999999</v>
@@ -8438,7 +8435,7 @@
         <v>119.26</v>
       </c>
       <c r="E301" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F301" t="s">
         <v>7</v>
@@ -8449,7 +8446,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C302">
         <v>119.26</v>
@@ -8458,7 +8455,7 @@
         <v>119.99</v>
       </c>
       <c r="E302" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F302" t="s">
         <v>7</v>
@@ -8469,7 +8466,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C303">
         <v>119.99</v>
@@ -8489,7 +8486,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C304">
         <v>120.94499999999999</v>
@@ -8509,7 +8506,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C305">
         <v>121.08499999999999</v>
@@ -8518,7 +8515,7 @@
         <v>121.255</v>
       </c>
       <c r="E305" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F305" t="s">
         <v>7</v>
@@ -8529,7 +8526,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C306">
         <v>121.255</v>
@@ -8538,7 +8535,7 @@
         <v>121.51</v>
       </c>
       <c r="E306" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F306" t="s">
         <v>7</v>
@@ -8549,7 +8546,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C307">
         <v>121.51</v>
@@ -8569,7 +8566,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C308">
         <v>121.66</v>
@@ -8578,7 +8575,7 @@
         <v>121.72499999999999</v>
       </c>
       <c r="E308" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F308" t="s">
         <v>7</v>
@@ -8589,7 +8586,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C309">
         <v>121.72499999999999</v>
@@ -8598,7 +8595,7 @@
         <v>122.49</v>
       </c>
       <c r="E309" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F309" t="s">
         <v>7</v>
@@ -8609,7 +8606,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C310">
         <v>122.49</v>
@@ -8629,7 +8626,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C311">
         <v>122.565</v>
@@ -8638,7 +8635,7 @@
         <v>122.795</v>
       </c>
       <c r="E311" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F311" t="s">
         <v>7</v>
@@ -8649,7 +8646,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C312">
         <v>122.795</v>
@@ -8658,7 +8655,7 @@
         <v>123.035</v>
       </c>
       <c r="E312" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F312" t="s">
         <v>7</v>
@@ -8669,7 +8666,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C313">
         <v>123.035</v>
@@ -8678,7 +8675,7 @@
         <v>123.035</v>
       </c>
       <c r="E313" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F313" t="s">
         <v>7</v>
@@ -8689,7 +8686,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C314">
         <v>123.035</v>
@@ -8698,7 +8695,7 @@
         <v>123.16</v>
       </c>
       <c r="E314" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F314" t="s">
         <v>7</v>
@@ -8709,7 +8706,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C315">
         <v>123.16</v>
@@ -8729,7 +8726,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C316">
         <v>123.23</v>
@@ -8738,7 +8735,7 @@
         <v>123.42</v>
       </c>
       <c r="E316" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F316" t="s">
         <v>7</v>
@@ -8749,7 +8746,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C317">
         <v>123.42</v>
@@ -8769,7 +8766,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C318">
         <v>125.125</v>
@@ -8778,7 +8775,7 @@
         <v>125.22499999999999</v>
       </c>
       <c r="E318" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F318" t="s">
         <v>7</v>
@@ -8789,7 +8786,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C319">
         <v>125.22499999999999</v>
@@ -8798,7 +8795,7 @@
         <v>125.52500000000001</v>
       </c>
       <c r="E319" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F319" t="s">
         <v>7</v>
@@ -8809,7 +8806,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C320">
         <v>125.52500000000001</v>
@@ -8818,7 +8815,7 @@
         <v>125.935</v>
       </c>
       <c r="E320" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F320" t="s">
         <v>7</v>
@@ -8829,7 +8826,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C321">
         <v>125.935</v>
@@ -8849,7 +8846,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C322">
         <v>126.29</v>
@@ -8858,7 +8855,7 @@
         <v>126.465</v>
       </c>
       <c r="E322" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F322" t="s">
         <v>7</v>
@@ -8869,7 +8866,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C323">
         <v>126.465</v>
@@ -8878,7 +8875,7 @@
         <v>126.77</v>
       </c>
       <c r="E323" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F323" t="s">
         <v>7</v>
@@ -8889,7 +8886,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C324">
         <v>126.77</v>
@@ -8898,7 +8895,7 @@
         <v>127.05500000000001</v>
       </c>
       <c r="E324" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F324" t="s">
         <v>7</v>
@@ -8909,7 +8906,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C325">
         <v>127.05500000000001</v>
@@ -8918,7 +8915,7 @@
         <v>127.27</v>
       </c>
       <c r="E325" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F325" t="s">
         <v>7</v>
@@ -8929,7 +8926,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C326">
         <v>127.27</v>
@@ -8938,7 +8935,7 @@
         <v>127.8</v>
       </c>
       <c r="E326" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F326" t="s">
         <v>7</v>

</xml_diff>